<commit_message>
Updates the CitationGecko classification with new found full-text papers
</commit_message>
<xml_diff>
--- a/output/citation_gecko/Recommendations_wb.xlsx
+++ b/output/citation_gecko/Recommendations_wb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mori.P16\OneDrive - UAM\Workspace\Multidimensional_parameters_MCLM\output\citation_gecko\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mori.P16\Documents\Workspace\mirt-parameters\output\citation_gecko\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="704">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -2115,37 +2115,22 @@
     <t>Derives a formula for the "angular direction" assuming othogonality (end of p. 399) but then does not assume orthogonality</t>
   </si>
   <si>
-    <t>Not relevant?</t>
-  </si>
-  <si>
-    <t>Review again: About "projection" to a unidimensional space, takes into account non-orthogonality when computing the projection but assumes orthogonality of the latent traits I think</t>
-  </si>
-  <si>
     <t>Deals with best measurement directions and composites, but the latent space axes of reference are assumed to be orthogonal</t>
   </si>
   <si>
-    <t>Review again: About "projection" to a unidimensional space, not sure whether it computes multidimensional discriminations or not</t>
-  </si>
-  <si>
-    <t>Está en Chino</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Check whether flexMirt computes correlated or only orthogonal dimensions</t>
-  </si>
-  <si>
     <t>Check this one in depth; it may be consdiering an orthogonal space even though the thetas are correlated</t>
   </si>
   <si>
-    <t>Oblique dimensions disregarding orthogonality?</t>
-  </si>
-  <si>
-    <t>Unclear: It mentions CFA in the method and results but does not give the correlation between latent traits; it speaks of "full-information item factor analysis" in the results, without specifying the method, so it is unclear whether the correlation was fixed to 0 or was estimated (but note the non-relevant discrimination parameters are fixed to 0)</t>
-  </si>
-  <si>
     <t>Simulates item discrimination parameters using the MDISC and cosines, but uses correlated simulated dimensions</t>
+  </si>
+  <si>
+    <t>In Chinese</t>
+  </si>
+  <si>
+    <t>The discussion mentions that the two latent traits were correlated, although it does not give an estimate of the correlation. It applies a MGRM and computes the MDISC (but not MDIFFs for each threshold); however, the solution has simple structure and therefore the MDISC is equal to the non-null discrimination parameter.</t>
+  </si>
+  <si>
+    <t>The three latent traits were correlated (Table 6). It computes the MDISC and  MDIFF; however, the solution has simple structure and therefore the MDISC is equal to the non-null discrimination parameter (and it does not affect the computation of the MDIFF).</t>
   </si>
 </sst>
 </file>
@@ -2500,16 +2485,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AI126" sqref="AI126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="32" max="32" width="216.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2684,28 +2671,25 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>1989</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="AI4" t="s">
         <v>689</v>
@@ -2713,28 +2697,31 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>1989</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>51</v>
       </c>
       <c r="AI5" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -2820,31 +2807,28 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>1992</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI9" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -2878,28 +2862,31 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>1992</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>72</v>
       </c>
       <c r="AI11" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
@@ -2958,7 +2945,7 @@
         <v>95</v>
       </c>
       <c r="AI12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -2984,7 +2971,7 @@
         <v>100</v>
       </c>
       <c r="AI13" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -3018,99 +3005,99 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B15">
         <v>1996</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
         <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
-      </c>
-      <c r="R15" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="T15" t="s">
         <v>111</v>
       </c>
       <c r="V15" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="AA15" t="s">
         <v>113</v>
       </c>
-      <c r="AB15" t="s">
-        <v>114</v>
-      </c>
       <c r="AC15" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="AD15" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="AF15" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="AI15" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>1996</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F16" t="s">
         <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>109</v>
+      </c>
+      <c r="R16" t="s">
+        <v>110</v>
       </c>
       <c r="T16" t="s">
         <v>111</v>
       </c>
       <c r="V16" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="AA16" t="s">
         <v>113</v>
       </c>
+      <c r="AB16" t="s">
+        <v>114</v>
+      </c>
       <c r="AC16" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AD16" t="s">
-        <v>125</v>
+        <v>116</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>117</v>
       </c>
       <c r="AF16" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="AI16" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -3173,57 +3160,57 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="B19">
         <v>1997</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F19" t="s">
         <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="AI19" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
       <c r="B20">
         <v>1997</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F20" t="s">
         <v>38</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>150</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>151</v>
       </c>
       <c r="AI20" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -3254,31 +3241,31 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>1997</v>
       </c>
       <c r="C22" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F22" t="s">
         <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="AF22" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="AI22" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -3338,28 +3325,28 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B25">
         <v>1999</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F25" t="s">
         <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="AF25" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="AI25" t="s">
         <v>689</v>
@@ -3367,28 +3354,28 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B26">
         <v>1999</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="E26" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F26" t="s">
         <v>38</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AF26" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="AI26" t="s">
         <v>689</v>
@@ -3507,28 +3494,28 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B30">
         <v>2001</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D30" t="s">
         <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="F30" t="s">
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="AF30" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="AI30" t="s">
         <v>689</v>
@@ -3536,28 +3523,28 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B31">
         <v>2001</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D31" t="s">
         <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F31" t="s">
         <v>38</v>
       </c>
       <c r="G31" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AF31" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="AI31" t="s">
         <v>689</v>
@@ -3682,86 +3669,86 @@
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="B35">
         <v>2003</v>
       </c>
       <c r="C35" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D35" t="s">
         <v>36</v>
       </c>
       <c r="E35" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="F35" t="s">
         <v>38</v>
       </c>
       <c r="G35" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="AF35" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="AI35" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="B36">
         <v>2003</v>
       </c>
       <c r="C36" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D36" t="s">
         <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F36" t="s">
         <v>38</v>
       </c>
       <c r="G36" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AF36" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="AI36" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B37">
         <v>2004</v>
       </c>
       <c r="C37" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>239</v>
       </c>
       <c r="E37" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="F37" t="s">
         <v>38</v>
       </c>
       <c r="G37" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="AF37" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="AI37" t="s">
         <v>689</v>
@@ -3769,31 +3756,34 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B38">
         <v>2004</v>
       </c>
       <c r="C38" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D38" t="s">
-        <v>239</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F38" t="s">
         <v>38</v>
       </c>
       <c r="G38" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="AF38" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="AI38" t="s">
         <v>689</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
@@ -3804,54 +3794,51 @@
         <v>2004</v>
       </c>
       <c r="C39" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>249</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F39" t="s">
         <v>38</v>
       </c>
       <c r="G39" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="AF39" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="AI39" t="s">
         <v>689</v>
-      </c>
-      <c r="AJ39" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B40">
         <v>2004</v>
       </c>
       <c r="C40" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D40" t="s">
-        <v>249</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
       </c>
       <c r="G40" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="AF40" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="AI40" t="s">
         <v>689</v>
@@ -3865,22 +3852,25 @@
         <v>2005</v>
       </c>
       <c r="C41" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D41" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E41" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F41" t="s">
         <v>38</v>
       </c>
       <c r="G41" t="s">
-        <v>256</v>
+        <v>260</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>261</v>
       </c>
       <c r="AI41" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
@@ -3891,199 +3881,196 @@
         <v>2005</v>
       </c>
       <c r="C42" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D42" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E42" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F42" t="s">
         <v>38</v>
       </c>
       <c r="G42" t="s">
-        <v>260</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="AI42" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="B43">
         <v>2005</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>179</v>
       </c>
       <c r="E43" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="F43" t="s">
         <v>38</v>
       </c>
       <c r="G43" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="AF43" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AI43" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>266</v>
+        <v>172</v>
       </c>
       <c r="B44">
         <v>2005</v>
       </c>
       <c r="C44" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D44" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="E44" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="F44" t="s">
         <v>38</v>
       </c>
       <c r="G44" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="AF44" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AI44" t="s">
-        <v>690</v>
+        <v>691</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>232</v>
       </c>
       <c r="B45">
         <v>2005</v>
       </c>
       <c r="C45" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E45" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="F45" t="s">
         <v>38</v>
       </c>
       <c r="G45" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="AF45" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="AI45" t="s">
-        <v>691</v>
-      </c>
-      <c r="AJ45" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B46">
         <v>2006</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
+        <v>249</v>
       </c>
       <c r="E46" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="F46" t="s">
         <v>38</v>
       </c>
       <c r="G46" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AF46" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="AI46" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B47">
         <v>2006</v>
       </c>
       <c r="C47" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D47" t="s">
-        <v>249</v>
+        <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F47" t="s">
         <v>38</v>
       </c>
       <c r="G47" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="AF47" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="AI47" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="B48">
         <v>2007</v>
       </c>
       <c r="C48" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E48" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="F48" t="s">
         <v>38</v>
       </c>
       <c r="G48" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="AF48" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="AI48" t="s">
         <v>689</v>
@@ -4120,179 +4107,179 @@
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="B50">
         <v>2007</v>
       </c>
       <c r="C50" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>300</v>
       </c>
       <c r="E50" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="F50" t="s">
         <v>38</v>
       </c>
       <c r="G50" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="AF50" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="AI50" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="B51">
         <v>2007</v>
       </c>
       <c r="C51" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="D51" t="s">
-        <v>300</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F51" t="s">
         <v>38</v>
       </c>
       <c r="G51" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="AF51" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="AI51" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B52">
         <v>2008</v>
       </c>
       <c r="C52" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D52" t="s">
         <v>249</v>
       </c>
       <c r="E52" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="F52" t="s">
         <v>38</v>
       </c>
       <c r="G52" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AF52" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="AI52" t="s">
         <v>691</v>
       </c>
       <c r="AJ52" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>309</v>
+        <v>197</v>
       </c>
       <c r="B53">
         <v>2008</v>
       </c>
       <c r="C53" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D53" t="s">
-        <v>249</v>
+        <v>98</v>
       </c>
       <c r="E53" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="F53" t="s">
         <v>38</v>
       </c>
       <c r="G53" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="AF53" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="AI53" t="s">
-        <v>691</v>
-      </c>
-      <c r="AJ53" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>304</v>
       </c>
       <c r="B54">
         <v>2008</v>
       </c>
       <c r="C54" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D54" t="s">
-        <v>98</v>
+        <v>249</v>
       </c>
       <c r="E54" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="F54" t="s">
         <v>38</v>
       </c>
       <c r="G54" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="AF54" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="AI54" t="s">
-        <v>689</v>
+        <v>691</v>
+      </c>
+      <c r="AJ54" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>275</v>
+        <v>365</v>
       </c>
       <c r="B55">
         <v>2009</v>
       </c>
       <c r="C55" t="s">
-        <v>318</v>
+        <v>366</v>
       </c>
       <c r="D55" t="s">
         <v>36</v>
       </c>
       <c r="E55" t="s">
-        <v>319</v>
+        <v>367</v>
       </c>
       <c r="F55" t="s">
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>320</v>
+        <v>368</v>
       </c>
       <c r="AF55" t="s">
-        <v>321</v>
+        <v>369</v>
       </c>
       <c r="AI55" t="s">
         <v>689</v>
@@ -4300,28 +4287,28 @@
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="B56">
         <v>2009</v>
       </c>
       <c r="C56" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D56" t="s">
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="F56" t="s">
         <v>38</v>
       </c>
       <c r="G56" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="AF56" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="AI56" t="s">
         <v>689</v>
@@ -4329,28 +4316,28 @@
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="B57">
         <v>2009</v>
       </c>
       <c r="C57" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="D57" t="s">
-        <v>42</v>
+        <v>347</v>
       </c>
       <c r="E57" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="F57" t="s">
         <v>38</v>
       </c>
       <c r="G57" t="s">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="AF57" t="s">
-        <v>331</v>
+        <v>350</v>
       </c>
       <c r="AI57" t="s">
         <v>689</v>
@@ -4358,28 +4345,28 @@
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>34</v>
+        <v>360</v>
       </c>
       <c r="B58">
         <v>2009</v>
       </c>
       <c r="C58" t="s">
-        <v>332</v>
+        <v>361</v>
       </c>
       <c r="D58" t="s">
-        <v>333</v>
+        <v>179</v>
       </c>
       <c r="E58" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="F58" t="s">
         <v>38</v>
       </c>
       <c r="G58" t="s">
-        <v>335</v>
+        <v>363</v>
       </c>
       <c r="AF58" t="s">
-        <v>336</v>
+        <v>364</v>
       </c>
       <c r="AI58" t="s">
         <v>689</v>
@@ -4387,60 +4374,57 @@
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>322</v>
       </c>
       <c r="B59">
         <v>2009</v>
       </c>
       <c r="C59" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="D59" t="s">
-        <v>333</v>
+        <v>42</v>
       </c>
       <c r="E59" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F59" t="s">
         <v>38</v>
       </c>
       <c r="G59" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="AF59" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="AI59" t="s">
-        <v>691</v>
-      </c>
-      <c r="AJ59" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>351</v>
       </c>
       <c r="B60">
         <v>2009</v>
       </c>
       <c r="C60" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="D60" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="E60" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="F60" t="s">
         <v>38</v>
       </c>
       <c r="G60" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="AF60" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="AI60" t="s">
         <v>689</v>
@@ -4448,28 +4432,28 @@
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B61">
         <v>2009</v>
       </c>
       <c r="C61" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D61" t="s">
-        <v>347</v>
+        <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="F61" t="s">
         <v>38</v>
       </c>
       <c r="G61" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="AF61" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="AI61" t="s">
         <v>689</v>
@@ -4477,28 +4461,28 @@
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>351</v>
+        <v>34</v>
       </c>
       <c r="B62">
         <v>2009</v>
       </c>
       <c r="C62" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="D62" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="E62" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="F62" t="s">
         <v>38</v>
       </c>
       <c r="G62" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="AF62" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="AI62" t="s">
         <v>689</v>
@@ -4506,28 +4490,28 @@
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>351</v>
+        <v>34</v>
       </c>
       <c r="B63">
         <v>2009</v>
       </c>
       <c r="C63" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>333</v>
       </c>
       <c r="E63" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="F63" t="s">
         <v>38</v>
       </c>
       <c r="G63" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="AF63" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="AI63" t="s">
         <v>689</v>
@@ -4535,57 +4519,60 @@
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>360</v>
+        <v>34</v>
       </c>
       <c r="B64">
         <v>2009</v>
       </c>
       <c r="C64" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="D64" t="s">
-        <v>179</v>
+        <v>333</v>
       </c>
       <c r="E64" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="F64" t="s">
         <v>38</v>
       </c>
       <c r="G64" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="AF64" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="AI64" t="s">
-        <v>689</v>
+        <v>691</v>
+      </c>
+      <c r="AJ64" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>365</v>
+        <v>275</v>
       </c>
       <c r="B65">
         <v>2009</v>
       </c>
       <c r="C65" t="s">
-        <v>366</v>
+        <v>318</v>
       </c>
       <c r="D65" t="s">
         <v>36</v>
       </c>
       <c r="E65" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
       <c r="F65" t="s">
         <v>38</v>
       </c>
       <c r="G65" t="s">
-        <v>368</v>
+        <v>320</v>
       </c>
       <c r="AF65" t="s">
-        <v>369</v>
+        <v>321</v>
       </c>
       <c r="AI65" t="s">
         <v>689</v>
@@ -4593,60 +4580,57 @@
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B66">
         <v>2010</v>
       </c>
       <c r="C66" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="D66" t="s">
-        <v>372</v>
+        <v>42</v>
       </c>
       <c r="E66" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="F66" t="s">
         <v>38</v>
       </c>
       <c r="G66" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="AF66" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="AI66" t="s">
-        <v>691</v>
-      </c>
-      <c r="AJ66" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="B67">
         <v>2010</v>
       </c>
       <c r="C67" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="E67" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="F67" t="s">
         <v>38</v>
       </c>
       <c r="G67" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="AF67" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="AI67" t="s">
         <v>689</v>
@@ -4654,124 +4638,121 @@
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="B68">
         <v>2010</v>
       </c>
       <c r="C68" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="D68" t="s">
-        <v>163</v>
+        <v>372</v>
       </c>
       <c r="E68" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="F68" t="s">
         <v>38</v>
       </c>
       <c r="G68" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="AF68" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="AI68" t="s">
-        <v>689</v>
+        <v>691</v>
+      </c>
+      <c r="AJ68" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>385</v>
+        <v>266</v>
       </c>
       <c r="B69">
         <v>2011</v>
       </c>
       <c r="C69" t="s">
-        <v>386</v>
+        <v>410</v>
       </c>
       <c r="D69" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E69" t="s">
-        <v>387</v>
+        <v>411</v>
       </c>
       <c r="F69" t="s">
         <v>38</v>
       </c>
       <c r="G69" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="AF69" t="s">
-        <v>389</v>
+        <v>413</v>
       </c>
       <c r="AI69" t="s">
-        <v>698</v>
-      </c>
-      <c r="AJ69" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>243</v>
+        <v>376</v>
       </c>
       <c r="B70">
         <v>2011</v>
       </c>
       <c r="C70" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="D70" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="E70" t="s">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="F70" t="s">
         <v>38</v>
       </c>
       <c r="G70" t="s">
-        <v>392</v>
+        <v>408</v>
       </c>
       <c r="AF70" t="s">
-        <v>393</v>
+        <v>409</v>
       </c>
       <c r="AI70" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>243</v>
+        <v>385</v>
       </c>
       <c r="B71">
         <v>2011</v>
       </c>
       <c r="C71" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="D71" t="s">
-        <v>179</v>
+        <v>36</v>
       </c>
       <c r="E71" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="F71" t="s">
         <v>38</v>
       </c>
       <c r="G71" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="AF71" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="AI71" t="s">
         <v>690</v>
-      </c>
-      <c r="AJ71" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
@@ -4834,86 +4815,89 @@
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>376</v>
+        <v>243</v>
       </c>
       <c r="B74">
         <v>2011</v>
       </c>
       <c r="C74" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="D74" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="E74" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="F74" t="s">
         <v>38</v>
       </c>
       <c r="G74" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="AF74" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="AI74" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="B75">
         <v>2011</v>
       </c>
       <c r="C75" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="D75" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="E75" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="F75" t="s">
         <v>38</v>
       </c>
       <c r="G75" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="AF75" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="AI75" t="s">
         <v>690</v>
       </c>
+      <c r="AJ75" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>232</v>
+        <v>424</v>
       </c>
       <c r="B76">
         <v>2012</v>
       </c>
       <c r="C76" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="D76" t="s">
         <v>42</v>
       </c>
       <c r="E76" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="F76" t="s">
         <v>38</v>
       </c>
       <c r="G76" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="AF76" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="AI76" t="s">
         <v>689</v>
@@ -4950,28 +4934,28 @@
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>424</v>
+        <v>275</v>
       </c>
       <c r="B78">
         <v>2012</v>
       </c>
       <c r="C78" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="D78" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="E78" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="F78" t="s">
         <v>38</v>
       </c>
       <c r="G78" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AF78" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="AI78" t="s">
         <v>689</v>
@@ -4979,28 +4963,28 @@
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="B79">
         <v>2012</v>
       </c>
       <c r="C79" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="D79" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="E79" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="F79" t="s">
         <v>38</v>
       </c>
       <c r="G79" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="AF79" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="AI79" t="s">
         <v>689</v>
@@ -5008,58 +4992,28 @@
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="B80">
         <v>2013</v>
       </c>
       <c r="C80" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="D80" t="s">
         <v>42</v>
       </c>
       <c r="E80" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="F80" t="s">
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>436</v>
-      </c>
-      <c r="R80" t="s">
-        <v>85</v>
-      </c>
-      <c r="T80" t="s">
-        <v>437</v>
-      </c>
-      <c r="V80" t="s">
-        <v>438</v>
-      </c>
-      <c r="AA80" t="s">
-        <v>439</v>
-      </c>
-      <c r="AB80" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC80" t="s">
-        <v>440</v>
-      </c>
-      <c r="AD80" t="s">
-        <v>441</v>
-      </c>
-      <c r="AE80" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="AF80" t="s">
-        <v>443</v>
-      </c>
-      <c r="AG80" t="s">
-        <v>444</v>
-      </c>
-      <c r="AH80" t="s">
-        <v>95</v>
+        <v>449</v>
       </c>
       <c r="AI80" t="s">
         <v>689</v>
@@ -5067,28 +5021,28 @@
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>445</v>
+        <v>376</v>
       </c>
       <c r="B81">
         <v>2013</v>
       </c>
       <c r="C81" t="s">
-        <v>446</v>
+        <v>463</v>
       </c>
       <c r="D81" t="s">
-        <v>42</v>
+        <v>249</v>
       </c>
       <c r="E81" t="s">
-        <v>447</v>
+        <v>464</v>
       </c>
       <c r="F81" t="s">
         <v>38</v>
       </c>
       <c r="G81" t="s">
-        <v>448</v>
+        <v>465</v>
       </c>
       <c r="AF81" t="s">
-        <v>449</v>
+        <v>466</v>
       </c>
       <c r="AI81" t="s">
         <v>689</v>
@@ -5096,28 +5050,28 @@
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="B82">
         <v>2013</v>
       </c>
       <c r="C82" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="D82" t="s">
         <v>249</v>
       </c>
       <c r="E82" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="F82" t="s">
         <v>38</v>
       </c>
       <c r="G82" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="AF82" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="AI82" t="s">
         <v>689</v>
@@ -5149,36 +5103,33 @@
         <v>457</v>
       </c>
       <c r="AI83" t="s">
-        <v>698</v>
-      </c>
-      <c r="AJ83" t="s">
-        <v>701</v>
+        <v>689</v>
       </c>
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>458</v>
+        <v>424</v>
       </c>
       <c r="B84">
         <v>2013</v>
       </c>
       <c r="C84" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D84" t="s">
         <v>249</v>
       </c>
       <c r="E84" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="F84" t="s">
         <v>38</v>
       </c>
       <c r="G84" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="AF84" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="AI84" t="s">
         <v>689</v>
@@ -5186,28 +5137,58 @@
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>376</v>
+        <v>433</v>
       </c>
       <c r="B85">
         <v>2013</v>
       </c>
       <c r="C85" t="s">
-        <v>463</v>
+        <v>434</v>
       </c>
       <c r="D85" t="s">
-        <v>249</v>
+        <v>42</v>
       </c>
       <c r="E85" t="s">
-        <v>464</v>
+        <v>435</v>
       </c>
       <c r="F85" t="s">
         <v>38</v>
       </c>
       <c r="G85" t="s">
-        <v>465</v>
+        <v>436</v>
+      </c>
+      <c r="R85" t="s">
+        <v>85</v>
+      </c>
+      <c r="T85" t="s">
+        <v>437</v>
+      </c>
+      <c r="V85" t="s">
+        <v>438</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>439</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>440</v>
+      </c>
+      <c r="AD85" t="s">
+        <v>441</v>
+      </c>
+      <c r="AE85" t="s">
+        <v>442</v>
       </c>
       <c r="AF85" t="s">
-        <v>466</v>
+        <v>443</v>
+      </c>
+      <c r="AG85" t="s">
+        <v>444</v>
+      </c>
+      <c r="AH85" t="s">
+        <v>95</v>
       </c>
       <c r="AI85" t="s">
         <v>689</v>
@@ -5299,89 +5280,92 @@
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="B89">
         <v>2015</v>
       </c>
       <c r="C89" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="D89" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="E89" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="F89" t="s">
         <v>38</v>
       </c>
       <c r="G89" t="s">
-        <v>483</v>
-      </c>
-      <c r="AF89" t="s">
-        <v>484</v>
+        <v>495</v>
       </c>
       <c r="AI89" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="AJ89" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B90">
         <v>2015</v>
       </c>
       <c r="C90" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="D90" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="E90" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="F90" t="s">
         <v>38</v>
       </c>
       <c r="G90" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="AF90" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="AI90" t="s">
         <v>689</v>
+      </c>
+      <c r="AJ90" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B91">
         <v>2015</v>
       </c>
       <c r="C91" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="D91" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="E91" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F91" t="s">
         <v>38</v>
       </c>
       <c r="G91" t="s">
-        <v>495</v>
+        <v>489</v>
+      </c>
+      <c r="AF91" t="s">
+        <v>490</v>
       </c>
       <c r="AI91" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
@@ -5415,118 +5399,112 @@
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="B93">
         <v>2015</v>
       </c>
       <c r="C93" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="D93" t="s">
-        <v>498</v>
+        <v>249</v>
       </c>
       <c r="E93" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="F93" t="s">
         <v>38</v>
       </c>
       <c r="G93" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="AF93" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="AI93" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B94">
         <v>2015</v>
       </c>
       <c r="C94" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D94" t="s">
-        <v>249</v>
+        <v>498</v>
       </c>
       <c r="E94" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="F94" t="s">
         <v>38</v>
       </c>
       <c r="G94" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="AF94" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="AI94" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>512</v>
+        <v>532</v>
       </c>
       <c r="B95">
         <v>2016</v>
       </c>
       <c r="C95" t="s">
-        <v>513</v>
+        <v>533</v>
       </c>
       <c r="D95" t="s">
-        <v>514</v>
+        <v>534</v>
       </c>
       <c r="E95" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="F95" t="s">
         <v>38</v>
       </c>
       <c r="G95" t="s">
-        <v>516</v>
-      </c>
-      <c r="AF95" t="s">
-        <v>517</v>
+        <v>536</v>
       </c>
       <c r="AI95" t="s">
-        <v>703</v>
-      </c>
-      <c r="AJ95" t="s">
-        <v>704</v>
+        <v>688</v>
       </c>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>424</v>
+        <v>527</v>
       </c>
       <c r="B96">
         <v>2016</v>
       </c>
       <c r="C96" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="D96" t="s">
-        <v>519</v>
+        <v>42</v>
       </c>
       <c r="E96" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="F96" t="s">
         <v>38</v>
       </c>
       <c r="G96" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
       <c r="AF96" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="AI96" t="s">
         <v>689</v>
@@ -5534,28 +5512,28 @@
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>502</v>
+        <v>537</v>
       </c>
       <c r="B97">
         <v>2016</v>
       </c>
       <c r="C97" t="s">
-        <v>523</v>
+        <v>538</v>
       </c>
       <c r="D97" t="s">
-        <v>42</v>
+        <v>539</v>
       </c>
       <c r="E97" t="s">
-        <v>524</v>
+        <v>540</v>
       </c>
       <c r="F97" t="s">
         <v>38</v>
       </c>
       <c r="G97" t="s">
-        <v>525</v>
+        <v>541</v>
       </c>
       <c r="AF97" t="s">
-        <v>526</v>
+        <v>542</v>
       </c>
       <c r="AI97" t="s">
         <v>689</v>
@@ -5563,28 +5541,28 @@
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>527</v>
+        <v>502</v>
       </c>
       <c r="B98">
         <v>2016</v>
       </c>
       <c r="C98" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="D98" t="s">
         <v>42</v>
       </c>
       <c r="E98" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="F98" t="s">
         <v>38</v>
       </c>
       <c r="G98" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="AF98" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="AI98" t="s">
         <v>689</v>
@@ -5592,115 +5570,115 @@
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>532</v>
+        <v>424</v>
       </c>
       <c r="B99">
         <v>2016</v>
       </c>
       <c r="C99" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="D99" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="E99" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="F99" t="s">
         <v>38</v>
       </c>
       <c r="G99" t="s">
-        <v>536</v>
+        <v>521</v>
+      </c>
+      <c r="AF99" t="s">
+        <v>522</v>
       </c>
       <c r="AI99" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>537</v>
+        <v>512</v>
       </c>
       <c r="B100">
         <v>2016</v>
       </c>
       <c r="C100" t="s">
-        <v>538</v>
+        <v>513</v>
       </c>
       <c r="D100" t="s">
-        <v>539</v>
+        <v>514</v>
       </c>
       <c r="E100" t="s">
-        <v>540</v>
+        <v>515</v>
       </c>
       <c r="F100" t="s">
         <v>38</v>
       </c>
       <c r="G100" t="s">
-        <v>541</v>
+        <v>516</v>
       </c>
       <c r="AF100" t="s">
-        <v>542</v>
+        <v>517</v>
       </c>
       <c r="AI100" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>543</v>
+        <v>167</v>
       </c>
       <c r="B101">
         <v>2017</v>
       </c>
       <c r="C101" t="s">
-        <v>544</v>
+        <v>568</v>
       </c>
       <c r="D101" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E101" t="s">
-        <v>545</v>
+        <v>569</v>
       </c>
       <c r="F101" t="s">
         <v>38</v>
       </c>
       <c r="G101" t="s">
-        <v>546</v>
+        <v>570</v>
       </c>
       <c r="AF101" t="s">
-        <v>547</v>
+        <v>571</v>
       </c>
       <c r="AI101" t="s">
-        <v>691</v>
-      </c>
-      <c r="AJ101" t="s">
-        <v>705</v>
+        <v>689</v>
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>479</v>
+        <v>572</v>
       </c>
       <c r="B102">
         <v>2017</v>
       </c>
       <c r="C102" t="s">
-        <v>548</v>
+        <v>573</v>
       </c>
       <c r="D102" t="s">
-        <v>481</v>
+        <v>574</v>
       </c>
       <c r="E102" t="s">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="F102" t="s">
         <v>38</v>
       </c>
       <c r="G102" t="s">
-        <v>550</v>
+        <v>576</v>
       </c>
       <c r="AF102" t="s">
-        <v>551</v>
+        <v>577</v>
       </c>
       <c r="AI102" t="s">
         <v>689</v>
@@ -5708,57 +5686,60 @@
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>243</v>
+        <v>543</v>
       </c>
       <c r="B103">
         <v>2017</v>
       </c>
       <c r="C103" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="D103" t="s">
-        <v>553</v>
+        <v>48</v>
       </c>
       <c r="E103" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="F103" t="s">
         <v>38</v>
       </c>
       <c r="G103" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="AF103" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="AI103" t="s">
-        <v>689</v>
+        <v>691</v>
+      </c>
+      <c r="AJ103" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="B104">
         <v>2017</v>
       </c>
       <c r="C104" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="D104" t="s">
-        <v>559</v>
+        <v>372</v>
       </c>
       <c r="E104" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="F104" t="s">
         <v>38</v>
       </c>
       <c r="G104" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="AF104" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="AI104" t="s">
         <v>689</v>
@@ -5766,28 +5747,28 @@
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B105">
         <v>2017</v>
       </c>
       <c r="C105" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D105" t="s">
-        <v>372</v>
+        <v>559</v>
       </c>
       <c r="E105" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="F105" t="s">
         <v>38</v>
       </c>
       <c r="G105" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="AF105" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="AI105" t="s">
         <v>689</v>
@@ -5795,28 +5776,28 @@
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>309</v>
       </c>
       <c r="B106">
         <v>2017</v>
       </c>
       <c r="C106" t="s">
-        <v>568</v>
+        <v>578</v>
       </c>
       <c r="D106" t="s">
-        <v>42</v>
+        <v>249</v>
       </c>
       <c r="E106" t="s">
-        <v>569</v>
+        <v>579</v>
       </c>
       <c r="F106" t="s">
         <v>38</v>
       </c>
       <c r="G106" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="AF106" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="AI106" t="s">
         <v>689</v>
@@ -5824,28 +5805,28 @@
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>572</v>
+        <v>479</v>
       </c>
       <c r="B107">
         <v>2017</v>
       </c>
       <c r="C107" t="s">
-        <v>573</v>
+        <v>548</v>
       </c>
       <c r="D107" t="s">
-        <v>574</v>
+        <v>481</v>
       </c>
       <c r="E107" t="s">
-        <v>575</v>
+        <v>549</v>
       </c>
       <c r="F107" t="s">
         <v>38</v>
       </c>
       <c r="G107" t="s">
-        <v>576</v>
+        <v>550</v>
       </c>
       <c r="AF107" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="AI107" t="s">
         <v>689</v>
@@ -5853,28 +5834,28 @@
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>309</v>
+        <v>243</v>
       </c>
       <c r="B108">
         <v>2017</v>
       </c>
       <c r="C108" t="s">
-        <v>578</v>
+        <v>552</v>
       </c>
       <c r="D108" t="s">
-        <v>249</v>
+        <v>553</v>
       </c>
       <c r="E108" t="s">
-        <v>579</v>
+        <v>554</v>
       </c>
       <c r="F108" t="s">
         <v>38</v>
       </c>
       <c r="G108" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
       <c r="AF108" t="s">
-        <v>581</v>
+        <v>556</v>
       </c>
       <c r="AI108" t="s">
         <v>689</v>
@@ -5882,28 +5863,55 @@
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
       <c r="B109">
         <v>2018</v>
       </c>
       <c r="C109" t="s">
-        <v>583</v>
+        <v>617</v>
       </c>
       <c r="D109" t="s">
-        <v>584</v>
+        <v>618</v>
       </c>
       <c r="E109" t="s">
-        <v>585</v>
+        <v>619</v>
       </c>
       <c r="F109" t="s">
         <v>38</v>
       </c>
       <c r="G109" t="s">
-        <v>586</v>
+        <v>620</v>
+      </c>
+      <c r="R109" t="s">
+        <v>621</v>
+      </c>
+      <c r="T109" t="s">
+        <v>622</v>
+      </c>
+      <c r="V109" t="s">
+        <v>623</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>624</v>
+      </c>
+      <c r="AB109" t="s">
+        <v>625</v>
+      </c>
+      <c r="AC109" t="s">
+        <v>626</v>
+      </c>
+      <c r="AD109" t="s">
+        <v>627</v>
       </c>
       <c r="AF109" t="s">
-        <v>587</v>
+        <v>628</v>
+      </c>
+      <c r="AG109" t="s">
+        <v>629</v>
+      </c>
+      <c r="AH109" t="s">
+        <v>95</v>
       </c>
       <c r="AI109" t="s">
         <v>691</v>
@@ -5911,118 +5919,118 @@
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>588</v>
+        <v>610</v>
       </c>
       <c r="B110">
         <v>2018</v>
       </c>
       <c r="C110" t="s">
-        <v>589</v>
+        <v>611</v>
       </c>
       <c r="D110" t="s">
-        <v>66</v>
+        <v>612</v>
       </c>
       <c r="E110" t="s">
-        <v>590</v>
+        <v>613</v>
       </c>
       <c r="F110" t="s">
         <v>38</v>
       </c>
       <c r="G110" t="s">
-        <v>591</v>
+        <v>614</v>
       </c>
       <c r="AF110" t="s">
-        <v>592</v>
+        <v>615</v>
       </c>
       <c r="AI110" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>512</v>
+        <v>598</v>
       </c>
       <c r="B111">
         <v>2018</v>
       </c>
       <c r="C111" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="D111" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="E111" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="F111" t="s">
         <v>38</v>
       </c>
       <c r="G111" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="AF111" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="AI111" t="s">
-        <v>690</v>
+        <v>691</v>
+      </c>
+      <c r="AJ111" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>598</v>
+        <v>582</v>
       </c>
       <c r="B112">
         <v>2018</v>
       </c>
       <c r="C112" t="s">
-        <v>599</v>
+        <v>583</v>
       </c>
       <c r="D112" t="s">
-        <v>600</v>
+        <v>584</v>
       </c>
       <c r="E112" t="s">
-        <v>601</v>
+        <v>585</v>
       </c>
       <c r="F112" t="s">
         <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
       <c r="AF112" t="s">
-        <v>603</v>
+        <v>587</v>
       </c>
       <c r="AI112" t="s">
-        <v>706</v>
-      </c>
-      <c r="AJ112" t="s">
-        <v>707</v>
+        <v>691</v>
       </c>
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>604</v>
+        <v>588</v>
       </c>
       <c r="B113">
         <v>2018</v>
       </c>
       <c r="C113" t="s">
-        <v>605</v>
+        <v>589</v>
       </c>
       <c r="D113" t="s">
-        <v>606</v>
+        <v>66</v>
       </c>
       <c r="E113" t="s">
-        <v>607</v>
+        <v>590</v>
       </c>
       <c r="F113" t="s">
         <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
       <c r="AF113" t="s">
-        <v>609</v>
+        <v>592</v>
       </c>
       <c r="AI113" t="s">
         <v>689</v>
@@ -6030,28 +6038,28 @@
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>610</v>
+        <v>512</v>
       </c>
       <c r="B114">
         <v>2018</v>
       </c>
       <c r="C114" t="s">
-        <v>611</v>
+        <v>593</v>
       </c>
       <c r="D114" t="s">
-        <v>612</v>
+        <v>594</v>
       </c>
       <c r="E114" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="F114" t="s">
         <v>38</v>
       </c>
       <c r="G114" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
       <c r="AF114" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
       <c r="AI114" t="s">
         <v>690</v>
@@ -6059,58 +6067,31 @@
     </row>
     <row r="115" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
       <c r="B115">
         <v>2018</v>
       </c>
       <c r="C115" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
       <c r="D115" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
       <c r="E115" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="F115" t="s">
         <v>38</v>
       </c>
       <c r="G115" t="s">
-        <v>620</v>
-      </c>
-      <c r="R115" t="s">
-        <v>621</v>
-      </c>
-      <c r="T115" t="s">
-        <v>622</v>
-      </c>
-      <c r="V115" t="s">
-        <v>623</v>
-      </c>
-      <c r="AA115" t="s">
-        <v>624</v>
-      </c>
-      <c r="AB115" t="s">
-        <v>625</v>
-      </c>
-      <c r="AC115" t="s">
-        <v>626</v>
-      </c>
-      <c r="AD115" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
       <c r="AF115" t="s">
-        <v>628</v>
-      </c>
-      <c r="AG115" t="s">
-        <v>629</v>
-      </c>
-      <c r="AH115" t="s">
-        <v>95</v>
+        <v>609</v>
       </c>
       <c r="AI115" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.25">
@@ -6144,60 +6125,57 @@
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="B117">
         <v>2019</v>
       </c>
       <c r="C117" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="D117" t="s">
-        <v>638</v>
+        <v>42</v>
       </c>
       <c r="E117" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="F117" t="s">
         <v>38</v>
       </c>
       <c r="G117" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="AF117" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="AI117" t="s">
-        <v>691</v>
-      </c>
-      <c r="AJ117" t="s">
-        <v>708</v>
+        <v>689</v>
       </c>
     </row>
     <row r="118" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="B118">
         <v>2019</v>
       </c>
       <c r="C118" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="D118" t="s">
         <v>42</v>
       </c>
       <c r="E118" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="F118" t="s">
         <v>38</v>
       </c>
       <c r="G118" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="AF118" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="AI118" t="s">
         <v>689</v>
@@ -6205,28 +6183,28 @@
     </row>
     <row r="119" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
       <c r="B119">
         <v>2019</v>
       </c>
       <c r="C119" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="D119" t="s">
-        <v>42</v>
+        <v>654</v>
       </c>
       <c r="E119" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="F119" t="s">
         <v>38</v>
       </c>
       <c r="G119" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="AF119" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="AI119" t="s">
         <v>689</v>
@@ -6234,86 +6212,89 @@
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="B120">
         <v>2019</v>
       </c>
       <c r="C120" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="D120" t="s">
-        <v>654</v>
+        <v>249</v>
       </c>
       <c r="E120" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="F120" t="s">
         <v>38</v>
       </c>
       <c r="G120" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="AF120" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
       <c r="AI120" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>658</v>
+        <v>636</v>
       </c>
       <c r="B121">
         <v>2019</v>
       </c>
       <c r="C121" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
       <c r="D121" t="s">
-        <v>249</v>
+        <v>638</v>
       </c>
       <c r="E121" t="s">
-        <v>660</v>
+        <v>639</v>
       </c>
       <c r="F121" t="s">
         <v>38</v>
       </c>
       <c r="G121" t="s">
-        <v>661</v>
+        <v>640</v>
       </c>
       <c r="AF121" t="s">
-        <v>662</v>
+        <v>641</v>
       </c>
       <c r="AI121" t="s">
-        <v>690</v>
+        <v>691</v>
+      </c>
+      <c r="AJ121" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="122" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>663</v>
+        <v>563</v>
       </c>
       <c r="B122">
         <v>2020</v>
       </c>
       <c r="C122" t="s">
-        <v>664</v>
+        <v>682</v>
       </c>
       <c r="D122" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="E122" t="s">
-        <v>665</v>
+        <v>683</v>
       </c>
       <c r="F122" t="s">
         <v>38</v>
       </c>
       <c r="G122" t="s">
-        <v>666</v>
+        <v>684</v>
       </c>
       <c r="AF122" t="s">
-        <v>667</v>
+        <v>685</v>
       </c>
       <c r="AI122" t="s">
         <v>689</v>
@@ -6321,28 +6302,28 @@
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="B123">
         <v>2020</v>
       </c>
       <c r="C123" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="D123" t="s">
-        <v>584</v>
+        <v>42</v>
       </c>
       <c r="E123" t="s">
-        <v>670</v>
+        <v>679</v>
       </c>
       <c r="F123" t="s">
         <v>38</v>
       </c>
       <c r="G123" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="AF123" t="s">
-        <v>672</v>
+        <v>681</v>
       </c>
       <c r="AI123" t="s">
         <v>689</v>
@@ -6350,95 +6331,99 @@
     </row>
     <row r="124" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>598</v>
+        <v>668</v>
       </c>
       <c r="B124">
         <v>2020</v>
       </c>
       <c r="C124" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D124" t="s">
-        <v>600</v>
+        <v>584</v>
       </c>
       <c r="E124" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="F124" t="s">
         <v>38</v>
       </c>
       <c r="G124" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="AF124" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="AI124" t="s">
-        <v>706</v>
-      </c>
-      <c r="AJ124" t="s">
-        <v>707</v>
+        <v>689</v>
       </c>
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>677</v>
+        <v>598</v>
       </c>
       <c r="B125">
         <v>2020</v>
       </c>
       <c r="C125" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="D125" t="s">
-        <v>42</v>
+        <v>600</v>
       </c>
       <c r="E125" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F125" t="s">
         <v>38</v>
       </c>
       <c r="G125" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="AF125" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="AI125" t="s">
-        <v>689</v>
+        <v>691</v>
+      </c>
+      <c r="AJ125" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>563</v>
+        <v>663</v>
       </c>
       <c r="B126">
         <v>2020</v>
       </c>
       <c r="C126" t="s">
-        <v>682</v>
+        <v>664</v>
       </c>
       <c r="D126" t="s">
-        <v>179</v>
+        <v>66</v>
       </c>
       <c r="E126" t="s">
-        <v>683</v>
+        <v>665</v>
       </c>
       <c r="F126" t="s">
         <v>38</v>
       </c>
       <c r="G126" t="s">
-        <v>684</v>
+        <v>666</v>
       </c>
       <c r="AF126" t="s">
-        <v>685</v>
+        <v>667</v>
       </c>
       <c r="AI126" t="s">
         <v>689</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:AJ126">
+    <sortCondition ref="B2:B126"/>
+    <sortCondition ref="A2:A126"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes in the classification of some papers, after reviewing them again in depth
</commit_message>
<xml_diff>
--- a/output/citation_gecko/Recommendations_wb.xlsx
+++ b/output/citation_gecko/Recommendations_wb.xlsx
@@ -2106,15 +2106,9 @@
     <t>Revise Case 1 (it may be "Not relevant", because it only uses multidimensional parameters in Case 2 where dimensions are set to be orthogonal)</t>
   </si>
   <si>
-    <t>Derives a formula for the "angular direction" assuming othogonality (end of p. 399) but then does not assume orthogonality</t>
-  </si>
-  <si>
     <t>Deals with best measurement directions and composites, but the latent space axes of reference are assumed to be orthogonal</t>
   </si>
   <si>
-    <t>Check this one in depth; it may be consdiering an orthogonal space even though the thetas are correlated</t>
-  </si>
-  <si>
     <t>Simulates item discrimination parameters using the MDISC and cosines, but uses correlated simulated dimensions</t>
   </si>
   <si>
@@ -2128,6 +2122,12 @@
   </si>
   <si>
     <t>Uses the MDISC and composite angle formulas to simulate the item parameters, disregarding the correlation among latent traits</t>
+  </si>
+  <si>
+    <t>Mentions the formula for the "angular direction" assuming othogonality (end of p. 399) but then does not assume orthogonality</t>
+  </si>
+  <si>
+    <t>Check this one in depth; it may be considering an orthogonal space even though the thetas are correlated</t>
   </si>
 </sst>
 </file>
@@ -2487,7 +2487,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="AI83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI94" sqref="AI94"/>
+      <selection pane="bottomRight" activeCell="AI100" sqref="AI100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4631,7 +4631,7 @@
         <v>689</v>
       </c>
       <c r="AJ67" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
@@ -4663,7 +4663,7 @@
         <v>689</v>
       </c>
       <c r="AJ68" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
@@ -5568,7 +5568,7 @@
         <v>691</v>
       </c>
       <c r="AJ99" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
@@ -5628,11 +5628,11 @@
       <c r="AF101" t="s">
         <v>375</v>
       </c>
-      <c r="AI101" t="s">
-        <v>691</v>
+      <c r="AI101" s="2" t="s">
+        <v>689</v>
       </c>
       <c r="AJ101" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
@@ -5751,7 +5751,7 @@
         <v>691</v>
       </c>
       <c r="AJ105" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
@@ -5839,7 +5839,7 @@
         <v>691</v>
       </c>
       <c r="AJ107" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
@@ -5900,7 +5900,7 @@
         <v>691</v>
       </c>
       <c r="AJ109" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
@@ -5932,7 +5932,7 @@
         <v>691</v>
       </c>
       <c r="AJ110" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
@@ -6295,7 +6295,7 @@
         <v>690</v>
       </c>
       <c r="AJ122" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates the classification of Tezza et al., 2018 (it must be "Oblique dimensions disregarding orthogonality")
</commit_message>
<xml_diff>
--- a/output/citation_gecko/Recommendations_wb.xlsx
+++ b/output/citation_gecko/Recommendations_wb.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="705">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -2103,9 +2103,6 @@
     <t>Mentions multidimensional discrimination in the discussion, but apparently it does not affect their results</t>
   </si>
   <si>
-    <t>Revise Case 1 (it may be "Not relevant", because it only uses multidimensional parameters in Case 2 where dimensions are set to be orthogonal)</t>
-  </si>
-  <si>
     <t>Deals with best measurement directions and composites, but the latent space axes of reference are assumed to be orthogonal</t>
   </si>
   <si>
@@ -2128,6 +2125,15 @@
   </si>
   <si>
     <t>Check this one in depth; it may be considering an orthogonal space even though the thetas are correlated</t>
+  </si>
+  <si>
+    <t>Case 1 uses the multidimensional parameters computed in Table 6.1.; see also chapter 6, section 6.2.1</t>
+  </si>
+  <si>
+    <t>Review again (MIRT model has correlated factors apparently, although not reported)</t>
+  </si>
+  <si>
+    <t>p. 927: "No presente estudo, a correlação entre a dimensão 1 e a dimensão 4 foi de aproximadamente 0,4"</t>
   </si>
 </sst>
 </file>
@@ -2484,10 +2490,10 @@
   <dimension ref="A1:AJ126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AI83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AI100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI100" sqref="AI100"/>
+      <selection pane="bottomRight" activeCell="AI105" sqref="AI105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4631,7 +4637,7 @@
         <v>689</v>
       </c>
       <c r="AJ67" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
@@ -4663,7 +4669,7 @@
         <v>689</v>
       </c>
       <c r="AJ68" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
@@ -5568,7 +5574,7 @@
         <v>691</v>
       </c>
       <c r="AJ99" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
@@ -5600,7 +5606,7 @@
         <v>691</v>
       </c>
       <c r="AJ100" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
@@ -5632,7 +5638,7 @@
         <v>689</v>
       </c>
       <c r="AJ101" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
@@ -5721,6 +5727,9 @@
       <c r="AI104" t="s">
         <v>691</v>
       </c>
+      <c r="AJ104" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -5751,7 +5760,7 @@
         <v>691</v>
       </c>
       <c r="AJ105" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
@@ -5839,7 +5848,7 @@
         <v>691</v>
       </c>
       <c r="AJ107" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
@@ -5900,7 +5909,7 @@
         <v>691</v>
       </c>
       <c r="AJ109" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
@@ -5932,7 +5941,7 @@
         <v>691</v>
       </c>
       <c r="AJ110" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
@@ -6295,7 +6304,7 @@
         <v>690</v>
       </c>
       <c r="AJ122" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
@@ -6382,7 +6391,10 @@
         <v>597</v>
       </c>
       <c r="AI125" t="s">
-        <v>690</v>
+        <v>691</v>
+      </c>
+      <c r="AJ125" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>